<commit_message>
Pom and Log files added
</commit_message>
<xml_diff>
--- a/TestProject/src/test/resources/Audi.xlsx
+++ b/TestProject/src/test/resources/Audi.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="267" yWindow="53" windowWidth="28227" windowHeight="14360"/>
+    <workbookView xWindow="0" yWindow="2373" windowWidth="20933" windowHeight="7893"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -63,9 +64,6 @@
     <t>PETROL</t>
   </si>
   <si>
-    <t>kX67 LFA</t>
-  </si>
-  <si>
     <t>AUDI</t>
   </si>
   <si>
@@ -76,6 +74,9 @@
   </si>
   <si>
     <t>102 g/km</t>
+  </si>
+  <si>
+    <t>KX67 LFA</t>
   </si>
 </sst>
 </file>
@@ -458,7 +459,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -523,13 +524,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="2">
         <v>42979</v>
@@ -538,10 +539,10 @@
         <v>2017</v>
       </c>
       <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added new java files and step definitions
</commit_message>
<xml_diff>
--- a/TestProject/src/test/resources/Audi.xlsx
+++ b/TestProject/src/test/resources/Audi.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2373" windowWidth="20933" windowHeight="7893"/>
+    <workbookView xWindow="-7" yWindow="3027" windowWidth="17080" windowHeight="3053"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CarDetails" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -86,16 +85,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,8 +116,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,36 +447,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.9375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.9375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.46875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.87890625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.29296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.9375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.8203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.9375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5859375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.46875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.87890625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.41015625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
@@ -532,7 +523,7 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>42979</v>
       </c>
       <c r="E2">

</xml_diff>

<commit_message>
Added more test data under Test Resources
</commit_message>
<xml_diff>
--- a/TestProject/src/test/resources/Audi.xlsx
+++ b/TestProject/src/test/resources/Audi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Vehicle make</t>
   </si>
@@ -27,36 +27,12 @@
     <t>Year of manufacture</t>
   </si>
   <si>
-    <t>Cylinder capacity (cc)</t>
-  </si>
-  <si>
-    <t>CO₂Emissions</t>
-  </si>
-  <si>
     <t>Fuel type</t>
   </si>
   <si>
-    <t>Euro Status</t>
-  </si>
-  <si>
-    <t>Export marker</t>
-  </si>
-  <si>
-    <t>Vehicle status</t>
-  </si>
-  <si>
     <t>Vehicle colour</t>
   </si>
   <si>
-    <t>Vehicle type approval</t>
-  </si>
-  <si>
-    <t>Wheelplan</t>
-  </si>
-  <si>
-    <t>Revenue weight</t>
-  </si>
-  <si>
     <t>Registration Number</t>
   </si>
   <si>
@@ -67,12 +43,6 @@
   </si>
   <si>
     <t>BLACK</t>
-  </si>
-  <si>
-    <t>999 cc</t>
-  </si>
-  <si>
-    <t>102 g/km</t>
   </si>
   <si>
     <t>KX67 LFA</t>
@@ -447,37 +417,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.29296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.234375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.9375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.8203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.9375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5859375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.46875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.87890625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.41015625" collapsed="true"/>
+    <col min="1" max="1" width="17.29296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.9375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.8203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.9375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -488,40 +451,16 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>42979</v>
@@ -530,13 +469,7 @@
         <v>2017</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>